<commit_message>
Atualização DR e cronograma
</commit_message>
<xml_diff>
--- a/02-Projeto/01-ResolveAi/01-GRE/02-PlanoGRE.xlsx
+++ b/02-Projeto/01-ResolveAi/01-GRE/02-PlanoGRE.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="7365" activeTab="1"/>
+    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="7365"/>
   </bookViews>
   <sheets>
     <sheet name="Tarefas" sheetId="2" r:id="rId1"/>
@@ -13,12 +13,12 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Papel</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Produtos</t>
   </si>
   <si>
-    <t>Iolanda, Matheus e Weverton</t>
-  </si>
-  <si>
     <t>Gerente de Requisitos</t>
   </si>
   <si>
@@ -125,13 +122,13 @@
     <t>Obter confirmação de entendimento e comprometimento dos requisitos com equipe técnica</t>
   </si>
   <si>
-    <t>Lista de comprometimento assinada</t>
-  </si>
-  <si>
     <t>Gerar baseline dos requisitos</t>
   </si>
   <si>
     <t>Baseline dos requisitos</t>
+  </si>
+  <si>
+    <t>Iolanda e Weverton</t>
   </si>
 </sst>
 </file>
@@ -264,7 +261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -293,17 +290,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -637,7 +637,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -662,99 +664,99 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="16">
+      <c r="A2" s="12">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="5" t="s">
+    </row>
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="15"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="15"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="13"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="13"/>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="12">
+        <v>2</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="11"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="11"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="12"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="12"/>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="16">
-        <v>2</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="10" t="s">
+    </row>
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="15"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="11"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="7" t="s">
+      <c r="D7" s="15"/>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="15"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="11"/>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="11"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="7" t="s">
+      <c r="D8" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="10" t="s">
+    </row>
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="13"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="9" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="12"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="11"/>
+      <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>3</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -762,41 +764,39 @@
         <v>4</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="5" t="s">
+    </row>
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="12">
+        <v>5</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="16">
-        <v>5</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="5" t="s">
+      <c r="D12" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="13"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="12"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>37</v>
-      </c>
+      <c r="D13" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="D6:D7"/>
@@ -806,6 +806,7 @@
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="A6:A9"/>
+    <mergeCell ref="D12:D13"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -815,7 +816,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -836,23 +839,23 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>